<commit_message>
distibutet data in 2 collums
</commit_message>
<xml_diff>
--- a/app-1 (todo)/files/archived_tasks.xlsx
+++ b/app-1 (todo)/files/archived_tasks.xlsx
@@ -9,6 +9,7 @@
     <sheet name="2024-08-17" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2024-08-18" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2024-08-19" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2024-08-20" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1263,4 +1264,37 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Archived Tasks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Continue 3H Of Python Cours</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: Update contact page layout and content
</commit_message>
<xml_diff>
--- a/app-1 (todo)/files/archived_tasks.xlsx
+++ b/app-1 (todo)/files/archived_tasks.xlsx
@@ -10,6 +10,7 @@
     <sheet name="2024-08-18" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2024-08-19" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2024-08-20" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2024-08-21" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1272,7 +1273,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1294,6 +1295,53 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Portfolio Website Done ✅</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Archived Tasks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Update Upwork Profile</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Fix Upwork To Show For Every Body</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor PDF generation code
</commit_message>
<xml_diff>
--- a/app-1 (todo)/files/archived_tasks.xlsx
+++ b/app-1 (todo)/files/archived_tasks.xlsx
@@ -11,6 +11,7 @@
     <sheet name="2024-08-19" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2024-08-20" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="2024-08-21" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2024-08-22" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1345,4 +1346,37 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Archived Tasks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1H Py Apps Course</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>